<commit_message>
Update replication study inventory and materials
Revised the replication study pool from 17 to 15 studies in the pre-analysis plan and updated the inventory workbook. Added and removed several published articles (PDFs) in the AEJ: Applied Economics, AJPS, and Psychological Science folders to reflect the new study selection. Updated auxiliary and log files to match the revised document structure and content.
</commit_message>
<xml_diff>
--- a/Papers/papers.xlsx
+++ b/Papers/papers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jposada/Library/CloudStorage/Dropbox/I4R/AI vertical/Papers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C79F18C-8B12-F445-8CD3-1E4FA179A088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E93F085-4F27-B147-8656-FC4AFBE53C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="51200" windowHeight="28180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="25600" windowHeight="28180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>Journal</t>
   </si>
@@ -46,12 +46,6 @@
     <t>Austerity, Economic Vulnerability, and Populism</t>
   </si>
   <si>
-    <t>Rain, Rain, Go Away: 194 Potential Exclusion‑Restriction Violations for Studies Using Weather as an Instrumental Variable</t>
-  </si>
-  <si>
-    <t>Differentially Private Survey Research</t>
-  </si>
-  <si>
     <t>A Spatial Rogowski Theory of America’s 19th‑Century Protectionism</t>
   </si>
   <si>
@@ -64,9 +58,6 @@
     <t>Expected Returns to Crime and Crime Location</t>
   </si>
   <si>
-    <t>Visual Short‑Term Memory Persists Across Multiple Fixations: An n‑Back Approach to Quantifying Capacity in Infants and Adults</t>
-  </si>
-  <si>
     <t>Universal Constraints on Linguistic Event Categories: A Cross‑Cultural Study of Child Homesign</t>
   </si>
   <si>
@@ -76,9 +67,6 @@
     <t>Contactless Real‑Time Heart Rate Predicts the Performance of Elite Athletes</t>
   </si>
   <si>
-    <t>Awe Sparks Prosociality in Children</t>
-  </si>
-  <si>
     <t>Impaired and Spared Auditory Category Learning in Developmental Dyslexia</t>
   </si>
   <si>
@@ -91,21 +79,12 @@
     <t>10.1111/ajps.12865</t>
   </si>
   <si>
-    <t>10.1111/ajps.12894</t>
-  </si>
-  <si>
-    <t>10.1111/ajps.12890</t>
-  </si>
-  <si>
     <t>10.1111/ajps.12870</t>
   </si>
   <si>
     <t>10.1257/app.20220279</t>
   </si>
   <si>
-    <t>10.1177/09567976221136509</t>
-  </si>
-  <si>
     <t>10.1177/09567976221140328</t>
   </si>
   <si>
@@ -115,9 +94,6 @@
     <t>10.1177/09567976221143127</t>
   </si>
   <si>
-    <t>10.1177/09567976221150616</t>
-  </si>
-  <si>
     <t>10.1177/09567976231151581</t>
   </si>
   <si>
@@ -130,12 +106,6 @@
     <t>https://doi.org/10.7910/DVN/1OPRYA</t>
   </si>
   <si>
-    <t>https://doi.org/10.7910/DVN/AQFTHK</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.7910/DVN/X4Y2FL</t>
-  </si>
-  <si>
     <t>https://doi.org/10.7910/DVN/PLKWUL</t>
   </si>
   <si>
@@ -169,9 +139,6 @@
     <t>https://www.openicpsr.org/openicpsr/project/190941/version/V1/view</t>
   </si>
   <si>
-    <t>https://osf.io/vfd2n/</t>
-  </si>
-  <si>
     <t>https://osf.io/jmv94</t>
   </si>
   <si>
@@ -181,9 +148,6 @@
     <t>https://osf.io/32jsy/</t>
   </si>
   <si>
-    <t>https://osf.io/8mv7h/</t>
-  </si>
-  <si>
     <t>https://doi.org/10.17605/OSF.IO/8QC24</t>
   </si>
   <si>
@@ -197,13 +161,31 @@
   </si>
   <si>
     <t>Replication Package URL</t>
+  </si>
+  <si>
+    <t>Biased bureaucrats and the policies of international organizations</t>
+  </si>
+  <si>
+    <t>10.1111/ajps.12921</t>
+  </si>
+  <si>
+    <t>Expertise Acquisition in Congress</t>
+  </si>
+  <si>
+    <t>10.1111/ajps.12848</t>
+  </si>
+  <si>
+    <t>https://dataverse.harvard.edu/dataset.xhtml?persistentId=doi:10.7910/DVN/VPPEAW</t>
+  </si>
+  <si>
+    <t>https://dataverse.harvard.edu/dataset.xhtml?persistentId=doi:10.7910/DVN/IPGCTN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,6 +197,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -252,17 +242,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -565,20 +560,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="98.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="98.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -595,299 +589,273 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2">
+        <v>2024</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>2024</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <v>2024</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5">
+        <v>2025</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6">
+        <v>2025</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B7">
         <v>2025</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>2024</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>2023</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>2023</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>2023</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>2023</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>2023</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>2023</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B15">
         <v>2024</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B16">
         <v>2024</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>2024</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="2">
-        <v>2024</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="2">
-        <v>2024</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="2">
-        <v>2024</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="C16" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="D16" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="E16" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E14">
+    <sortCondition ref="A1:A14"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="E16" r:id="rId1" xr:uid="{98DD7861-FFFA-8C46-B79A-A2DF08746BCD}"/>
+    <hyperlink ref="E15" r:id="rId2" xr:uid="{2AED3BD5-DB2B-0F4F-A94E-A4EBE60B5E05}"/>
+    <hyperlink ref="E14" r:id="rId3" xr:uid="{4C7920B4-5FDE-4646-9F29-804FE3F90E86}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>